<commit_message>
excel_writer: switch to English
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_download_iuvo_statement_no_cfs.xlsx
+++ b/tests/expected_results/result_test_download_iuvo_statement_no_cfs.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,10 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>